<commit_message>
Zzy 24 01 08 (#531)
* [REF] MOQ分摊成本转列为行

* [ADD] BOM成本处材料单价原币、汇率、材料单价人民币、合计金额人民币含客供、不含客供、损耗、材料成本含损耗，保留5位小数的逻辑

* [REF] 时效性查询时间显示逻辑

* [REF] 更改核价表标题

* [REF] 更改名称错误修复

* [REF] 年份

---------

Co-authored-by: wszhuzy <wszhuzy@sunnyoptical.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/SolutionContrast.xlsx
+++ b/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/SolutionContrast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\代码\财务\二开\后端\finance_back\aspnet-core\src\Finance.Web.Host\wwwroot\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0871F71-7F52-4FE8-B503-F7197F2C7901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB42B001-2881-47BF-8322-106BB669D374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>{{Name1}}</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -132,116 +132,6 @@
   </si>
   <si>
     <t>方案1项目名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>方案</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>MOQ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>分摊成本</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>方案</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>MOQ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>分摊成本</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{SolutionContrast.MoqShareCount_2}}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{SolutionContrast.MoqShareCount_1}}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -647,18 +537,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="13" width="20" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -668,22 +558,20 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
+      <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -695,30 +583,24 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -732,40 +614,34 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>